<commit_message>
A bunch of Images and Results
A bunch of Images and Results in xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Results.xlsx
+++ b/Documentation/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sskal\OneDrive\Documents\GitHub\SimulatedDistributedSystems\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0460C192-DBBD-4287-8DDC-1442D91C28FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA29BAC-A4F7-4BCC-9D65-228DA1E3FA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7E584F17-1EE3-41F7-BE14-DF1EEE38F655}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Total Time (ms)</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>Average (s)</t>
+  </si>
+  <si>
+    <t>Time (ms)</t>
+  </si>
+  <si>
+    <t>Total Time (ns)</t>
+  </si>
+  <si>
+    <t>Average (ms)</t>
   </si>
 </sst>
 </file>
@@ -159,12 +168,6 @@
               <a:rPr lang="en-US" baseline="0"/>
               <a:t>(Problematic Architecture)</a:t>
             </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US" baseline="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -782,7 +785,725 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Query Time of Microservices  </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>(Improved Architecture)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Improved!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Improved!$B$2:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Improved!$C$2:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>0.63190000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60619999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66020000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.72109999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64410000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.60150000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55110000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56759999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.54659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.7710999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.84340000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.52290000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.59370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.60070000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.55989999999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.56899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.72719999999999996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.70220000000000005</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.50649999999999995</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.47239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.75209999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.75209999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.65590000000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.49080000000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.59160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.87680000000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.46700000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-06F1-485B-AF6B-B683F6DFA206}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1743012015"/>
+        <c:axId val="1743012495"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1743012015"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Query</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1743012495"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1743012495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time(ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1743012015"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1338,6 +2059,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1359,6 +2596,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6944E8B7-9347-38B8-9CA5-CE3A8BFE5519}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>195262</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD58B664-722C-ACB8-C165-701A13D89C85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1702,7 +2980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE1C76C-4C1D-4825-8692-27C31329899A}">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="N8" sqref="N8:O9"/>
     </sheetView>
   </sheetViews>
@@ -2107,12 +3385,406 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60123096-593A-4FB6-A837-E17F9317DA50}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>631900</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>A2/(1000000)</f>
+        <v>0.63190000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>606200</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C31" si="0">A3/(1000000)</f>
+        <v>0.60619999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>686000</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.68600000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>751900</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.75190000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>660200</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.66020000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>721100</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.72109999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>644100</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.64410000000000001</v>
+      </c>
+      <c r="M8" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <f>AVERAGE(C2:C31)</f>
+        <v>0.68078666666666654</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>601500</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.60150000000000003</v>
+      </c>
+      <c r="M9" t="s">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <f>STDEV(C2:C31)</f>
+        <v>0.23989631917564558</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>551100</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.55110000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>567600</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0.56759999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>546600</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0.54659999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1771100</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1.7710999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>843400</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0.84340000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1000100</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1.0001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>522900</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>0.52290000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>593700</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>0.59370000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>600700</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>0.60070000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>559900</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0.55989999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>569000</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0.56899999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>727200</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0.72719999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>702200</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0.70220000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>506500</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>0.50649999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>472400</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>0.47239999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>752100</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>0.75209999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>752100</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>0.75209999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>655900</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>0.65590000000000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>490800</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>0.49080000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>591600</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>0.59160000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>876800</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>0.87680000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>467000</f>
+        <v>467000</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>0.46700000000000003</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>